<commit_message>
Crates + climb & patrol behaviour
</commit_message>
<xml_diff>
--- a/PD - Log File - Crimson Skies.xlsx
+++ b/PD - Log File - Crimson Skies.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
   <si>
     <t>Day</t>
   </si>
@@ -92,6 +92,36 @@
   </si>
   <si>
     <t>Build rough level with Probuilder &amp; Find and insert free water shader</t>
+  </si>
+  <si>
+    <t>Wingtip smoke particle system</t>
+  </si>
+  <si>
+    <t>Primary gunnery system, particles &amp; sound</t>
+  </si>
+  <si>
+    <t>Refine particle system for wing smoke</t>
+  </si>
+  <si>
+    <t>Groundwork for AI dogfighting, calculating steering</t>
+  </si>
+  <si>
+    <t>AI framework</t>
+  </si>
+  <si>
+    <t>Tweaking AI</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>AI firing logic + 1st order intercept</t>
+  </si>
+  <si>
+    <t>Hit detection + fix sound</t>
+  </si>
+  <si>
+    <t>Enemy plane model + camera swivel</t>
   </si>
 </sst>
 </file>
@@ -398,7 +428,7 @@
       </c>
       <c r="I1" s="3">
         <f>SUM(E2:E55)</f>
-        <v>0.7986111111</v>
+        <v>1.319444444</v>
       </c>
     </row>
     <row r="2">
@@ -759,84 +789,192 @@
       </c>
     </row>
     <row r="19">
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
+      <c r="A19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="4">
+        <v>44686.0</v>
+      </c>
+      <c r="C19" s="5">
+        <v>0.4479166666666667</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0.4791666666666667</v>
+      </c>
       <c r="E19" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.03125</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="20">
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
+      <c r="A20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="4">
+        <v>44686.0</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0.4791666666666667</v>
+      </c>
+      <c r="D20" s="5">
+        <v>0.53125</v>
+      </c>
       <c r="E20" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.05208333333</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="21">
-      <c r="B21" s="7"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
+      <c r="A21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="4">
+        <v>6691369.0</v>
+      </c>
+      <c r="C21" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0.7916666666666666</v>
+      </c>
       <c r="E21" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.04166666667</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="22">
-      <c r="B22" s="7"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
+      <c r="A22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="4">
+        <v>44687.0</v>
+      </c>
+      <c r="C22" s="6">
+        <v>0.4166666666666667</v>
+      </c>
+      <c r="D22" s="5">
+        <v>0.5</v>
+      </c>
       <c r="E22" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.08333333333</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="23">
-      <c r="B23" s="7"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
+      <c r="A23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="4">
+        <v>44687.0</v>
+      </c>
+      <c r="C23" s="5">
+        <v>0.5625</v>
+      </c>
+      <c r="D23" s="5">
+        <v>0.625</v>
+      </c>
       <c r="E23" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.0625</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="24">
-      <c r="B24" s="7"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
+      <c r="A24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="4">
+        <v>44687.0</v>
+      </c>
+      <c r="C24" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="D24" s="5">
+        <v>0.7916666666666666</v>
+      </c>
       <c r="E24" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.04166666667</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="25">
-      <c r="B25" s="7"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
+      <c r="A25" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="4">
+        <v>44688.0</v>
+      </c>
+      <c r="C25" s="6">
+        <v>0.4583333333333333</v>
+      </c>
+      <c r="D25" s="5">
+        <v>0.5208333333333334</v>
+      </c>
       <c r="E25" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.0625</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="26">
-      <c r="B26" s="7"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
+      <c r="A26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="4">
+        <v>44693.0</v>
+      </c>
+      <c r="C26" s="6">
+        <v>0.5833333333333334</v>
+      </c>
+      <c r="D26" s="5">
+        <v>0.6666666666666666</v>
+      </c>
       <c r="E26" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.08333333333</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="27">
-      <c r="B27" s="7"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
+      <c r="A27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="4">
+        <v>44693.0</v>
+      </c>
+      <c r="C27" s="6">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="D27" s="5">
+        <v>0.7291666666666666</v>
+      </c>
       <c r="E27" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.0625</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="28">

</xml_diff>

<commit_message>
:sparkles: final content commit
</commit_message>
<xml_diff>
--- a/PD - Log File - Crimson Skies.xlsx
+++ b/PD - Log File - Crimson Skies.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="46">
   <si>
     <t>Day</t>
   </si>
@@ -122,6 +122,33 @@
   </si>
   <si>
     <t>Enemy plane model + camera swivel</t>
+  </si>
+  <si>
+    <t>Secondary Weapon: Missile + Health and Ammo crates</t>
+  </si>
+  <si>
+    <t>Dogfighting endurance and 1/2 level climb</t>
+  </si>
+  <si>
+    <t>2/2 Level climb + Patrol behaviour</t>
+  </si>
+  <si>
+    <t>Level progression: Cinematic Door opening 1/2</t>
+  </si>
+  <si>
+    <t>Level progression: Cinematic Door opening 2/2</t>
+  </si>
+  <si>
+    <t>Enemy trackers on player HUD</t>
+  </si>
+  <si>
+    <t>Enemy trackers: out of camera behaviour + level sculpting</t>
+  </si>
+  <si>
+    <t>Balance pass for health, damage and speed</t>
+  </si>
+  <si>
+    <t>Handin work</t>
   </si>
 </sst>
 </file>
@@ -427,8 +454,8 @@
         <v>6</v>
       </c>
       <c r="I1" s="3">
-        <f>SUM(E2:E55)</f>
-        <v>1.319444444</v>
+        <f>SUM(E2:E65)</f>
+        <v>1.986111111</v>
       </c>
     </row>
     <row r="2">
@@ -445,7 +472,7 @@
         <v>0.4791666666666667</v>
       </c>
       <c r="E2" s="3">
-        <f t="shared" ref="E2:E31" si="1">D2-C2</f>
+        <f t="shared" ref="E2:E47" si="1">D2-C2</f>
         <v>0.02083333333</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -940,7 +967,7 @@
         <v>12</v>
       </c>
       <c r="B26" s="4">
-        <v>44693.0</v>
+        <v>44692.0</v>
       </c>
       <c r="C26" s="6">
         <v>0.5833333333333334</v>
@@ -961,7 +988,7 @@
         <v>12</v>
       </c>
       <c r="B27" s="4">
-        <v>44693.0</v>
+        <v>44692.0</v>
       </c>
       <c r="C27" s="6">
         <v>0.6666666666666666</v>
@@ -978,120 +1005,292 @@
       </c>
     </row>
     <row r="28">
-      <c r="B28" s="7"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
+      <c r="A28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="4">
+        <v>44693.0</v>
+      </c>
+      <c r="C28" s="5">
+        <v>0.4479166666666667</v>
+      </c>
+      <c r="D28" s="5">
+        <v>0.53125</v>
+      </c>
       <c r="E28" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.08333333333</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="29">
-      <c r="B29" s="7"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
+      <c r="A29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="4">
+        <v>44694.0</v>
+      </c>
+      <c r="C29" s="5">
+        <v>0.3958333333333333</v>
+      </c>
+      <c r="D29" s="5">
+        <v>0.4583333333333333</v>
+      </c>
       <c r="E29" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.0625</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="30">
-      <c r="B30" s="7"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
+      <c r="A30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="4">
+        <v>44699.0</v>
+      </c>
+      <c r="C30" s="5">
+        <v>0.5625</v>
+      </c>
+      <c r="D30" s="5">
+        <v>0.6041666666666666</v>
+      </c>
       <c r="E30" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.04166666667</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="31">
-      <c r="B31" s="7"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
+      <c r="A31" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="4">
+        <v>44700.0</v>
+      </c>
+      <c r="C31" s="6">
+        <v>0.4166666666666667</v>
+      </c>
+      <c r="D31" s="6">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="E31" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.125</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="32">
-      <c r="B32" s="7"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
+      <c r="A32" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="4">
+        <v>44707.0</v>
+      </c>
+      <c r="C32" s="5">
+        <v>0.4166666666666667</v>
+      </c>
+      <c r="D32" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E32" s="3">
+        <f t="shared" si="1"/>
+        <v>0.08333333333</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="33">
-      <c r="B33" s="7"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
+      <c r="A33" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="4">
+        <v>44707.0</v>
+      </c>
+      <c r="C33" s="6">
+        <v>0.5833333333333334</v>
+      </c>
+      <c r="D33" s="6">
+        <v>0.7083333333333334</v>
+      </c>
+      <c r="E33" s="3">
+        <f t="shared" si="1"/>
+        <v>0.125</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="34">
-      <c r="B34" s="7"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
+      <c r="A34" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="4">
+        <v>44708.0</v>
+      </c>
+      <c r="C34" s="6">
+        <v>0.4166666666666667</v>
+      </c>
+      <c r="D34" s="5">
+        <v>0.5208333333333334</v>
+      </c>
+      <c r="E34" s="3">
+        <f t="shared" si="1"/>
+        <v>0.1041666667</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="35">
-      <c r="B35" s="7"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
+      <c r="A35" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="4">
+        <v>44708.0</v>
+      </c>
+      <c r="C35" s="5">
+        <v>0.625</v>
+      </c>
+      <c r="D35" s="5">
+        <v>0.6458333333333334</v>
+      </c>
+      <c r="E35" s="3">
+        <f t="shared" si="1"/>
+        <v>0.02083333333</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="36">
-      <c r="B36" s="7"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
+      <c r="A36" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="4">
+        <v>44708.0</v>
+      </c>
+      <c r="C36" s="5">
+        <v>0.6458333333333334</v>
+      </c>
+      <c r="D36" s="5">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="E36" s="3">
+        <f t="shared" si="1"/>
+        <v>0.02083333333</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="37">
       <c r="B37" s="7"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
+      <c r="E37" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="B38" s="7"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
+      <c r="E38" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="B39" s="7"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
+      <c r="E39" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="B40" s="7"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
+      <c r="E40" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="41">
       <c r="B41" s="7"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
+      <c r="E41" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="B42" s="7"/>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
+      <c r="E42" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="B43" s="7"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
+      <c r="E43" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="B44" s="7"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
+      <c r="E44" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="B45" s="7"/>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
+      <c r="E45" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="B46" s="7"/>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
+      <c r="E46" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="B47" s="7"/>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
+      <c r="E47" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="B48" s="7"/>

</xml_diff>